<commit_message>
update add img and video to server
</commit_message>
<xml_diff>
--- a/data/regrester.xlsx
+++ b/data/regrester.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
   <si>
     <t>No</t>
   </si>
@@ -86,7 +86,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="37" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +163,158 @@
       <b val="true"/>
       <color indexed="9"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="61">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -217,8 +367,258 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="123">
     <border>
       <left/>
       <right/>
@@ -386,12 +786,462 @@
       <top style="medium"/>
       <bottom style="medium"/>
     </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="52">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
@@ -440,7 +1290,32 @@
     <xf applyBorder="true" applyFill="true" borderId="10" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="14" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="18" fillId="8" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="22" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="22" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="26" fillId="12" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="30" fillId="14" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="34" fillId="16" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="38" fillId="18" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="42" fillId="20" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="46" fillId="22" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="50" fillId="24" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="54" fillId="26" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="58" fillId="28" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="62" fillId="30" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="66" fillId="32" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="70" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="74" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="78" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="82" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="86" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="90" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="94" fillId="46" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="98" fillId="48" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="102" fillId="50" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="106" fillId="52" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="110" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="114" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="118" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="60" borderId="122" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -722,7 +1597,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:AI7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="E11" sqref="E11"/>
@@ -799,9 +1674,81 @@
       <c r="I2" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21"/>
+      <c r="J2" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="U2" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="V2" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="W2" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y2" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z2" s="43" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA2" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC2" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD2" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="AE2" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF2" s="49" t="s">
+        <v>17</v>
+      </c>
+      <c r="AG2" s="50" t="s">
+        <v>17</v>
+      </c>
+      <c r="AH2" s="51" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>

</xml_diff>

<commit_message>
update insters report to server
</commit_message>
<xml_diff>
--- a/data/regrester.xlsx
+++ b/data/regrester.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
   <si>
     <t>No</t>
   </si>
@@ -86,7 +86,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="49" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,8 +313,80 @@
       <b val="true"/>
       <color indexed="9"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+      <color indexed="9"/>
+    </font>
   </fonts>
-  <fills count="61">
+  <fills count="85">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -617,8 +689,128 @@
         <bgColor indexed="2"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor indexed="2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="123">
+  <borders count="171">
     <border>
       <left/>
       <right/>
@@ -1236,12 +1428,228 @@
       <top style="medium"/>
       <bottom style="medium"/>
     </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
     <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="6" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="64">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
@@ -1315,7 +1723,19 @@
     <xf applyBorder="true" applyFill="true" borderId="110" fillId="54" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="114" fillId="56" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="118" fillId="58" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="60" borderId="122" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="122" fillId="60" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="126" fillId="62" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="130" fillId="64" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="134" fillId="66" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="138" fillId="68" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="142" fillId="70" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="146" fillId="72" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="150" fillId="74" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="154" fillId="76" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="158" fillId="78" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="162" fillId="80" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="166" fillId="82" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="84" borderId="170" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
@@ -1597,7 +2017,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AU7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="E11" sqref="E11"/>
@@ -1747,6 +2167,42 @@
         <v>17</v>
       </c>
       <c r="AH2" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="AI2" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ2" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK2" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL2" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="AM2" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN2" s="57" t="s">
+        <v>17</v>
+      </c>
+      <c r="AO2" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="AP2" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="AQ2" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="AR2" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="AS2" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="AT2" s="63" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>